<commit_message>
added page cross over documentation and test updates
</commit_message>
<xml_diff>
--- a/bck-up/page_cross_over.xlsx
+++ b/bck-up/page_cross_over.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="133">
   <si>
     <t xml:space="preserve">ROW</t>
   </si>
@@ -101,6 +102,1444 @@
   </si>
   <si>
     <t xml:space="preserve">00170FAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programmed Addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase Addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FF0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3FC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111100</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">FC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3FD</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111101</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">FD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3FE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111110</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">FE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3FF</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111111</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">FF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000000</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000001</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">402</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000010</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">403</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000011</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10FF4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43FD</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111101</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">43FE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111110</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">43FF</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111111</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">4400</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000000</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">4401</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000001</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">4402</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000010</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">4403</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000011</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">4404</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000100</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4405</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000101</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4406</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000110</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4407</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000111</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4408</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00001000</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4409</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00001001</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">440A</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00001010</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">0A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">440B</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00001011</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">0B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">440C</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00001100</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">0C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20FF8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83FE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111110</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">83FF</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111111</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">8400</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000000</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">8401</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000001</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">8402</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000010</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">8403</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000011</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">8404</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000100</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">8405</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000101</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">8406</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000110</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">8407</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000111</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">8408</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00001000</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">8409</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00001001</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">840A</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00001010</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">840B</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00001011</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">840C</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00001100</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">840D</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED1C24"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00001101</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">0D</t>
   </si>
 </sst>
 </file>
@@ -110,7 +1549,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -132,6 +1571,27 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00A65D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0066B3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFED1C24"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -220,7 +1680,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -273,6 +1733,42 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -286,7 +1782,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFED1C24"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -306,7 +1802,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF0066B3"/>
       <rgbColor rgb="FFD6DCE5"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -333,7 +1829,7 @@
       <rgbColor rgb="FF5565AF"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00A65D"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -352,8 +1848,8 @@
   </sheetPr>
   <dimension ref="D1:AK1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6:X6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2366,4 +3862,894 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G46"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="14.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="14" t="n">
+        <v>7</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="15" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="15" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="15" t="n">
+        <v>10</v>
+      </c>
+      <c r="F15" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="F16" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="F17" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="F18" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="F19" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="14" t="n">
+        <v>7</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="F20" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="14" t="n">
+        <v>8</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="F21" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="14" t="n">
+        <v>9</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="F22" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="F23" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="F24" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="14" t="n">
+        <v>12</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="F25" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="F26" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="14" t="n">
+        <v>14</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="F27" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="14" t="n">
+        <v>15</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="F28" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="14"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="F31" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="F32" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E33" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F33" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F34" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F35" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E36" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F36" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F37" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="14" t="n">
+        <v>7</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F38" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="14" t="n">
+        <v>8</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F39" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="14" t="n">
+        <v>9</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E40" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F40" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F41" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F42" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="14" t="n">
+        <v>12</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="E43" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F43" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E44" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F44" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="14" t="n">
+        <v>14</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E45" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F45" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="14" t="n">
+        <v>15</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E46" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F46" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated WB  Rule 3.00 assert
</commit_message>
<xml_diff>
--- a/bck-up/page_cross_over.xlsx
+++ b/bck-up/page_cross_over.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="random results" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="154">
   <si>
     <t xml:space="preserve">ROW</t>
   </si>
@@ -1540,6 +1541,301 @@
   </si>
   <si>
     <t xml:space="preserve">0D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73FFE8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01CFFFA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'11100111111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111010</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">73F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01CFFFB</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'11100111111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111011</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">FB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01CFFFC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'11100111111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111100</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">01CFFFD</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'11100111111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111101</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">01CFFFE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'11100111111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111110</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">01CFFFF</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'11100111111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11111111</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">01D0000</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'11101000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000000</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">01D0001</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'11101000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0066B3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00000001</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">01cfffa</t>
   </si>
 </sst>
 </file>
@@ -1549,7 +1845,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1589,6 +1885,19 @@
     <font>
       <sz val="11"/>
       <color rgb="FFED1C24"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE181E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1680,7 +1989,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1769,6 +2078,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1832,7 +2145,7 @@
       <rgbColor rgb="FF00A65D"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFCE181E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -1849,7 +2162,7 @@
   <dimension ref="D1:AK1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3871,8 +4184,8 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3880,7 +4193,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="14.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="17.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.23"/>
@@ -4741,6 +5054,231 @@
       </c>
       <c r="G46" s="20" t="s">
         <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B3:M13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="G7" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="G10" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="15" t="n">
+        <v>740</v>
+      </c>
+      <c r="G11" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="14" t="n">
+        <v>7</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" s="15" t="n">
+        <v>740</v>
+      </c>
+      <c r="G12" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M13" s="0" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>